<commit_message>
atualizacao banco, arquivo esquematico fonte
</commit_message>
<xml_diff>
--- a/relatorio/despesas.xlsx
+++ b/relatorio/despesas.xlsx
@@ -139,7 +139,7 @@
     <xf numFmtId="42" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
@@ -196,6 +196,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -388,7 +389,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
@@ -436,7 +437,7 @@
       <c r="B3" s="11" t="n"/>
       <c r="C3" s="9" t="inlineStr">
         <is>
-          <t>Retorno: None</t>
+          <t>Retorno: 2025-07-03</t>
         </is>
       </c>
       <c r="D3" s="11" t="n"/>
@@ -506,58 +507,58 @@
     <row r="9" ht="17.35" customFormat="1" customHeight="1" s="6">
       <c r="A9" s="14" t="inlineStr">
         <is>
-          <t>bar e restaurante dona nilza</t>
+          <t>igor dezem rafaine - brodowski</t>
         </is>
       </c>
       <c r="B9" s="14" t="inlineStr">
         <is>
-          <t>26/06/2025 12:16</t>
+          <t>23/06/2025 08:19</t>
         </is>
       </c>
       <c r="C9" s="15">
-        <f>hyperlink("notas fiscal/20250626_121759.jpg", "20250626_121759.jpg")</f>
+        <f>hyperlink("notas fiscal/20250623_082034.jpg", "20250623_082034.jpg")</f>
         <v/>
       </c>
       <c r="D9" s="16" t="n">
-        <v>30.51</v>
+        <v>10.99</v>
       </c>
     </row>
     <row r="10" ht="17.35" customFormat="1" customHeight="1" s="6">
       <c r="A10" s="14" t="inlineStr">
         <is>
-          <t>igor dezem rafaine - brodowski</t>
+          <t>comercial iguatemi ltda- me</t>
         </is>
       </c>
       <c r="B10" s="14" t="inlineStr">
         <is>
-          <t>23/06/2025 08:19</t>
+          <t>23/06/2025 10:04</t>
         </is>
       </c>
       <c r="C10" s="15">
-        <f>hyperlink("notas fiscal/20250623_082034.jpg", "20250623_082034.jpg")</f>
+        <f>hyperlink("notas fiscal/20250623_100731.jpg", "20250623_100731.jpg")</f>
         <v/>
       </c>
       <c r="D10" s="16" t="n">
-        <v>10.99</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" ht="17.35" customFormat="1" customHeight="1" s="6">
       <c r="A11" s="14" t="inlineStr">
         <is>
-          <t>comercial iguatemi ltda- me</t>
+          <t>panificadora amigos ltda</t>
         </is>
       </c>
       <c r="B11" s="14" t="inlineStr">
         <is>
-          <t>23/06/2025 10:04</t>
+          <t>24/06/2025 07:36</t>
         </is>
       </c>
       <c r="C11" s="15">
-        <f>hyperlink("notas fiscal/20250623_100731.jpg", "20250623_100731.jpg")</f>
+        <f>hyperlink("notas fiscal/20250624_073800_1yl5PSC.jpg", "20250624_073800_1yl5PSC.jpg")</f>
         <v/>
       </c>
       <c r="D11" s="16" t="n">
-        <v>16</v>
+        <v>14.5</v>
       </c>
     </row>
     <row r="12" ht="17.35" customFormat="1" customHeight="1" s="6">
@@ -568,53 +569,53 @@
       </c>
       <c r="B12" s="14" t="inlineStr">
         <is>
-          <t>27/06/2025 12:14</t>
+          <t>24/06/2025 12:22</t>
         </is>
       </c>
       <c r="C12" s="15">
-        <f>hyperlink("notas fiscal/20250628_085259.jpg", "20250628_085259.jpg")</f>
+        <f>hyperlink("notas fiscal/20250628_090221.jpg", "20250628_090221.jpg")</f>
         <v/>
       </c>
       <c r="D12" s="16" t="n">
-        <v>32.49</v>
+        <v>27.5</v>
       </c>
     </row>
     <row r="13" ht="17.35" customFormat="1" customHeight="1" s="6">
       <c r="A13" s="14" t="inlineStr">
         <is>
-          <t>bar e restaurante dona nilza</t>
+          <t>dma distribuidora s/a</t>
         </is>
       </c>
       <c r="B13" s="14" t="inlineStr">
         <is>
-          <t>24/06/2025 12:22</t>
+          <t>24/06/2025 17:46</t>
         </is>
       </c>
       <c r="C13" s="15">
-        <f>hyperlink("notas fiscal/20250628_090221.jpg", "20250628_090221.jpg")</f>
+        <f>hyperlink("notas fiscal/20250624_184701.jpg", "20250624_184701.jpg")</f>
         <v/>
       </c>
       <c r="D13" s="16" t="n">
-        <v>27.5</v>
+        <v>29.78</v>
       </c>
     </row>
     <row r="14" ht="17.35" customFormat="1" customHeight="1" s="6">
       <c r="A14" s="14" t="inlineStr">
         <is>
-          <t>panificadora amigos ltda</t>
+          <t>bar e restaurante dona nilza</t>
         </is>
       </c>
       <c r="B14" s="14" t="inlineStr">
         <is>
-          <t>24/06/2025 07:36</t>
+          <t>25/06/2025 12:51</t>
         </is>
       </c>
       <c r="C14" s="15">
-        <f>hyperlink("notas fiscal/20250624_073800_1yl5PSC.jpg", "20250624_073800_1yl5PSC.jpg")</f>
+        <f>hyperlink("notas fiscal/20250625_125327.jpg", "20250625_125327.jpg")</f>
         <v/>
       </c>
       <c r="D14" s="16" t="n">
-        <v>14.5</v>
+        <v>32.49</v>
       </c>
     </row>
     <row r="15" ht="17.35" customFormat="1" customHeight="1" s="6">
@@ -625,91 +626,91 @@
       </c>
       <c r="B15" s="14" t="inlineStr">
         <is>
-          <t>25/06/2025 12:51</t>
+          <t>26/06/2025 12:16</t>
         </is>
       </c>
       <c r="C15" s="15">
-        <f>hyperlink("notas fiscal/20250625_125327.jpg", "20250625_125327.jpg")</f>
+        <f>hyperlink("notas fiscal/20250626_121759.jpg", "20250626_121759.jpg")</f>
         <v/>
       </c>
       <c r="D15" s="16" t="n">
-        <v>32.49</v>
+        <v>30.51</v>
       </c>
     </row>
     <row r="16" ht="17.35" customFormat="1" customHeight="1" s="6">
       <c r="A16" s="14" t="inlineStr">
         <is>
-          <t>jaqueline oliveira de melo</t>
+          <t>lanchonete sabor e saúde</t>
         </is>
       </c>
       <c r="B16" s="14" t="inlineStr">
         <is>
-          <t>28/06/2025 12:26</t>
+          <t>26/06/2025 18:00</t>
         </is>
       </c>
       <c r="C16" s="15">
-        <f>hyperlink("notas fiscal/20250623_122829.jpg", "20250623_122829.jpg")</f>
+        <f>hyperlink("notas fiscal/20250626_211609_pT9iyyC.jpg", "20250626_211609_pT9iyyC.jpg")</f>
         <v/>
       </c>
       <c r="D16" s="16" t="n">
-        <v>21.22</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="17" ht="17.35" customFormat="1" customHeight="1" s="6">
       <c r="A17" s="14" t="inlineStr">
         <is>
-          <t>dma distribuidora s/a</t>
+          <t>bar e restaurante dona nilza</t>
         </is>
       </c>
       <c r="B17" s="14" t="inlineStr">
         <is>
-          <t>24/06/2025 17:46</t>
+          <t>27/06/2025 12:14</t>
         </is>
       </c>
       <c r="C17" s="15">
-        <f>hyperlink("notas fiscal/20250624_184701.jpg", "20250624_184701.jpg")</f>
+        <f>hyperlink("notas fiscal/20250628_085259.jpg", "20250628_085259.jpg")</f>
         <v/>
       </c>
       <c r="D17" s="16" t="n">
-        <v>29.78</v>
+        <v>32.49</v>
       </c>
     </row>
     <row r="18" ht="17.35" customFormat="1" customHeight="1" s="6">
       <c r="A18" s="14" t="inlineStr">
         <is>
-          <t>lanchonete sabor e saúde</t>
+          <t>mercado bh, mercado epa,  ifood</t>
         </is>
       </c>
       <c r="B18" s="14" t="inlineStr">
         <is>
-          <t>26/06/2025 18:00</t>
+          <t>27/06/2025 20:14</t>
         </is>
       </c>
       <c r="C18" s="15">
-        <f>hyperlink("notas fiscal/20250626_211609_pT9iyyC.jpg", "20250626_211609_pT9iyyC.jpg")</f>
+        <f>hyperlink("notas fiscal/IMG-20250628-WA0004.jpg", "IMG-20250628-WA0004.jpg")</f>
         <v/>
       </c>
       <c r="D18" s="16" t="n">
-        <v>6.5</v>
+        <v>268.89</v>
       </c>
     </row>
     <row r="19" ht="17.35" customFormat="1" customHeight="1" s="6">
       <c r="A19" s="14" t="inlineStr">
         <is>
-          <t>mercado bh, mercado epa,  ifood</t>
+          <t>jaqueline oliveira de melo</t>
         </is>
       </c>
       <c r="B19" s="14" t="inlineStr">
         <is>
-          <t>27/06/2025 20:14</t>
+          <t>28/06/2025 12:26</t>
         </is>
       </c>
       <c r="C19" s="15">
-        <f>hyperlink("notas fiscal/IMG-20250628-WA0004.jpg", "IMG-20250628-WA0004.jpg")</f>
+        <f>hyperlink("notas fiscal/20250623_122829.jpg", "20250623_122829.jpg")</f>
         <v/>
       </c>
       <c r="D19" s="16" t="n">
-        <v>268.89</v>
+        <v>21.22</v>
       </c>
     </row>
     <row r="20" ht="17.35" customFormat="1" customHeight="1" s="6">
@@ -751,106 +752,150 @@
       </c>
     </row>
     <row r="22" ht="17.35" customHeight="1" s="8">
-      <c r="A22" s="17" t="inlineStr">
-        <is>
-          <t>TOTAL</t>
-        </is>
-      </c>
-      <c r="B22" s="18" t="n"/>
-      <c r="C22" s="18" t="n"/>
-      <c r="D22" s="14">
-        <f>sum(D9:D21)</f>
-        <v/>
+      <c r="A22" s="14" t="inlineStr">
+        <is>
+          <t>bar e restaurante dona nilza</t>
+        </is>
+      </c>
+      <c r="B22" s="14" t="inlineStr">
+        <is>
+          <t>30/06/2025 12:34</t>
+        </is>
+      </c>
+      <c r="C22" s="15">
+        <f>hyperlink("notas fiscal/20250630_123543.jpg", "20250630_123543.jpg")</f>
+        <v/>
+      </c>
+      <c r="D22" s="16" t="n">
+        <v>31</v>
       </c>
     </row>
     <row r="23" ht="17.35" customHeight="1" s="8">
-      <c r="A23" s="19" t="n"/>
-      <c r="B23" s="19" t="n"/>
-      <c r="C23" s="19" t="n"/>
-      <c r="D23" s="19" t="n"/>
+      <c r="A23" s="14" t="inlineStr">
+        <is>
+          <t>jantar</t>
+        </is>
+      </c>
+      <c r="B23" s="14" t="inlineStr">
+        <is>
+          <t>30/06/2025 20:06</t>
+        </is>
+      </c>
+      <c r="C23" s="15">
+        <f>hyperlink("notas fiscal/IMG-20250701-WA0017.jpg", "IMG-20250701-WA0017.jpg")</f>
+        <v/>
+      </c>
+      <c r="D23" s="16" t="n">
+        <v>31.65</v>
+      </c>
     </row>
     <row r="24" ht="17.35" customHeight="1" s="8">
-      <c r="A24" s="17" t="inlineStr">
-        <is>
-          <t>Descricão Do Adiantamento</t>
-        </is>
-      </c>
-      <c r="B24" s="18" t="n"/>
-      <c r="C24" s="18" t="n"/>
-      <c r="D24" s="18" t="n"/>
+      <c r="A24" s="14" t="inlineStr">
+        <is>
+          <t>bar e restaurante dona nilza</t>
+        </is>
+      </c>
+      <c r="B24" s="14" t="inlineStr">
+        <is>
+          <t>01/07/2025 12:37</t>
+        </is>
+      </c>
+      <c r="C24" s="15">
+        <f>hyperlink("notas fiscal/20250702_232526.jpg", "20250702_232526.jpg")</f>
+        <v/>
+      </c>
+      <c r="D24" s="16" t="n">
+        <v>25.02</v>
+      </c>
     </row>
     <row r="25" ht="17.35" customHeight="1" s="8">
-      <c r="A25" s="17" t="inlineStr">
-        <is>
-          <t>Descrição</t>
-        </is>
-      </c>
-      <c r="B25" s="17" t="inlineStr">
-        <is>
-          <t>Data</t>
-        </is>
-      </c>
-      <c r="C25" s="17" t="inlineStr">
-        <is>
-          <t>Comprovante</t>
-        </is>
-      </c>
-      <c r="D25" s="17" t="inlineStr">
-        <is>
-          <t>Value</t>
-        </is>
+      <c r="A25" s="14" t="inlineStr">
+        <is>
+          <t>churrascaria boi na brasa</t>
+        </is>
+      </c>
+      <c r="B25" s="14" t="inlineStr">
+        <is>
+          <t>02/07/2025 06:44</t>
+        </is>
+      </c>
+      <c r="C25" s="15">
+        <f>hyperlink("notas fiscal/20250702_230555.jpg", "20250702_230555.jpg")</f>
+        <v/>
+      </c>
+      <c r="D25" s="16" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="26" ht="17.35" customHeight="1" s="8">
       <c r="A26" s="14" t="inlineStr">
         <is>
-          <t>transferencia recebida</t>
+          <t>doces queijos iguatemy</t>
         </is>
       </c>
       <c r="B26" s="14" t="inlineStr">
         <is>
-          <t>20/06/2025 08:49</t>
+          <t>02/07/2025 07:19</t>
         </is>
       </c>
       <c r="C26" s="15">
-        <f>hyperlink("notas fiscal/IMG-20250629-WA0010_ux4VgRy.jpg", "IMG-20250629-WA0010_ux4VgRy.jpg")</f>
+        <f>hyperlink("notas fiscal/20250702_230408.jpg", "20250702_230408.jpg")</f>
         <v/>
       </c>
       <c r="D26" s="16" t="n">
-        <v>800</v>
+        <v>73.04000000000001</v>
       </c>
     </row>
     <row r="27" ht="17.35" customHeight="1" s="8">
-      <c r="A27" s="19" t="n"/>
-      <c r="B27" s="19" t="n"/>
-      <c r="C27" s="19" t="n"/>
-      <c r="D27" s="19" t="n"/>
+      <c r="A27" s="14" t="inlineStr">
+        <is>
+          <t>restaurante cazulao</t>
+        </is>
+      </c>
+      <c r="B27" s="14" t="inlineStr">
+        <is>
+          <t>02/07/2025 10:48</t>
+        </is>
+      </c>
+      <c r="C27" s="15">
+        <f>hyperlink("notas fiscal/20250702_225912_ASJ9Sfd.jpg", "20250702_225912_ASJ9Sfd.jpg")</f>
+        <v/>
+      </c>
+      <c r="D27" s="16" t="n">
+        <v>18</v>
+      </c>
     </row>
     <row r="28" ht="17.35" customHeight="1" s="8">
-      <c r="A28" s="17" t="inlineStr">
-        <is>
-          <t>Receber</t>
-        </is>
-      </c>
-      <c r="B28" s="18" t="n"/>
-      <c r="C28" s="17" t="inlineStr">
-        <is>
-          <t>Devolver</t>
-        </is>
-      </c>
-      <c r="D28" s="18" t="n"/>
+      <c r="A28" s="14" t="inlineStr">
+        <is>
+          <t>churrascaria tucuman ltda</t>
+        </is>
+      </c>
+      <c r="B28" s="14" t="inlineStr">
+        <is>
+          <t>02/07/2025 13:52</t>
+        </is>
+      </c>
+      <c r="C28" s="15">
+        <f>hyperlink("notas fiscal/20250702_225517.jpg", "20250702_225517.jpg")</f>
+        <v/>
+      </c>
+      <c r="D28" s="16" t="n">
+        <v>23.9</v>
+      </c>
     </row>
     <row r="29" ht="17.35" customHeight="1" s="8">
-      <c r="A29" s="16">
-        <f>if(sum(D26:D26) - D22 &lt;0, D22 - sum(D26:D26), 0)</f>
-        <v/>
+      <c r="A29" s="17" t="inlineStr">
+        <is>
+          <t>TOTAL</t>
+        </is>
       </c>
       <c r="B29" s="18" t="n"/>
-      <c r="C29" s="16">
-        <f>if(sum(D26:D26) - D22&lt;0, 0, sum(D26:D26) -  D22)</f>
-        <v/>
-      </c>
-      <c r="D29" s="18" t="n"/>
+      <c r="C29" s="18" t="n"/>
+      <c r="D29" s="14">
+        <f>sum(D9:D28)</f>
+        <v/>
+      </c>
     </row>
     <row r="30" ht="17.35" customHeight="1" s="8">
       <c r="A30" s="19" t="n"/>
@@ -859,33 +904,74 @@
       <c r="D30" s="19" t="n"/>
     </row>
     <row r="31" ht="17.35" customHeight="1" s="8">
-      <c r="A31" s="19" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Apucarana, 29 de junho de 2025 </t>
-        </is>
-      </c>
+      <c r="A31" s="17" t="inlineStr">
+        <is>
+          <t>Descricão Do Adiantamento</t>
+        </is>
+      </c>
+      <c r="B31" s="18" t="n"/>
+      <c r="C31" s="18" t="n"/>
+      <c r="D31" s="18" t="n"/>
     </row>
     <row r="32" ht="17.35" customHeight="1" s="8">
-      <c r="A32" s="19" t="n"/>
-      <c r="B32" s="19" t="n"/>
-      <c r="C32" s="19" t="n"/>
-      <c r="D32" s="19" t="n"/>
+      <c r="A32" s="17" t="inlineStr">
+        <is>
+          <t>Descrição</t>
+        </is>
+      </c>
+      <c r="B32" s="17" t="inlineStr">
+        <is>
+          <t>Data</t>
+        </is>
+      </c>
+      <c r="C32" s="17" t="inlineStr">
+        <is>
+          <t>Comprovante</t>
+        </is>
+      </c>
+      <c r="D32" s="17" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
     </row>
     <row r="33" ht="17.35" customHeight="1" s="8">
-      <c r="A33" s="19" t="inlineStr">
-        <is>
-          <t>__________________________________</t>
-        </is>
-      </c>
-      <c r="C33" s="19" t="inlineStr">
-        <is>
-          <t>__________________________________</t>
-        </is>
+      <c r="A33" s="14" t="inlineStr">
+        <is>
+          <t>transferencia recebida</t>
+        </is>
+      </c>
+      <c r="B33" s="14" t="inlineStr">
+        <is>
+          <t>20/06/2025 08:49</t>
+        </is>
+      </c>
+      <c r="C33" s="15">
+        <f>hyperlink("notas fiscal/IMG-20250629-WA0010_ux4VgRy.jpg", "IMG-20250629-WA0010_ux4VgRy.jpg")</f>
+        <v/>
+      </c>
+      <c r="D33" s="16" t="n">
+        <v>800</v>
       </c>
     </row>
     <row r="34" ht="17.35" customHeight="1" s="8">
-      <c r="A34" s="19" t="n"/>
-      <c r="C34" s="19" t="n"/>
+      <c r="A34" s="14" t="inlineStr">
+        <is>
+          <t>transferencia recebida</t>
+        </is>
+      </c>
+      <c r="B34" s="14" t="inlineStr">
+        <is>
+          <t>30/06/2025 11:05</t>
+        </is>
+      </c>
+      <c r="C34" s="15">
+        <f>hyperlink("notas fiscal/IMG-20250701-WA0016_eCzmQzQ.jpg", "IMG-20250701-WA0016_eCzmQzQ.jpg")</f>
+        <v/>
+      </c>
+      <c r="D34" s="16" t="n">
+        <v>700</v>
+      </c>
     </row>
     <row r="35" ht="17.35" customHeight="1" s="8">
       <c r="A35" s="19" t="n"/>
@@ -894,32 +980,72 @@
       <c r="D35" s="19" t="n"/>
     </row>
     <row r="36" ht="17.35" customHeight="1" s="8">
-      <c r="A36" s="19" t="n"/>
-      <c r="B36" s="19" t="n"/>
-      <c r="C36" s="19" t="n"/>
-      <c r="D36" s="19" t="n"/>
-    </row>
+      <c r="A36" s="17" t="inlineStr">
+        <is>
+          <t>Receber</t>
+        </is>
+      </c>
+      <c r="B36" s="18" t="n"/>
+      <c r="C36" s="17" t="inlineStr">
+        <is>
+          <t>Devolver</t>
+        </is>
+      </c>
+      <c r="D36" s="18" t="n"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="20">
+        <f>if(sum(D33:D34) - D29 &lt;0, D29 - sum(D33:D34), 0)</f>
+        <v/>
+      </c>
+      <c r="B37" s="18" t="n"/>
+      <c r="C37" s="20">
+        <f>if(sum(D33:D34) - D29&lt;0, 0, sum(D33:D34) -  D29)</f>
+        <v/>
+      </c>
+      <c r="D37" s="18" t="n"/>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Apucarana, 03 de julho de 2025 </t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>__________________________________</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>__________________________________</t>
+        </is>
+      </c>
+    </row>
+    <row r="42"/>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="A36:B36"/>
     <mergeCell ref="A31:D31"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="A39:D39"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A29:C29"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A33:B33"/>
     <mergeCell ref="B4:D4"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="C36:D36"/>
     <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C37:D37"/>
     <mergeCell ref="C3:D3"/>
-    <mergeCell ref="A34:B34"/>
   </mergeCells>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7875" right="0.7875" top="0.886111111111111" bottom="0.886111111111111" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Adcionado funcionalidade de extrai dados da url da nota fiscal
</commit_message>
<xml_diff>
--- a/relatorio/despesas.xlsx
+++ b/relatorio/despesas.xlsx
@@ -139,7 +139,7 @@
     <xf numFmtId="42" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
@@ -196,7 +196,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -389,7 +388,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
@@ -437,7 +436,7 @@
       <c r="B3" s="11" t="n"/>
       <c r="C3" s="9" t="inlineStr">
         <is>
-          <t>Retorno: 2025-07-03</t>
+          <t>Retorno: None</t>
         </is>
       </c>
       <c r="D3" s="11" t="n"/>
@@ -445,12 +444,12 @@
     <row r="4" ht="14.45" customHeight="1" s="8">
       <c r="A4" s="9" t="inlineStr">
         <is>
-          <t>Destino: Contagem - MG</t>
+          <t>Destino: Curitiba - PR</t>
         </is>
       </c>
       <c r="B4" s="9" t="inlineStr">
         <is>
-          <t>Motivo Viagem: Implantação DRL Parte 2</t>
+          <t>Motivo Viagem: Instalação Contabilista</t>
         </is>
       </c>
       <c r="C4" s="10" t="n"/>
@@ -507,395 +506,213 @@
     <row r="9" ht="17.35" customFormat="1" customHeight="1" s="6">
       <c r="A9" s="14" t="inlineStr">
         <is>
-          <t>igor dezem rafaine - brodowski</t>
+          <t>marqueze casaril e cia ltda</t>
         </is>
       </c>
       <c r="B9" s="14" t="inlineStr">
         <is>
-          <t>23/06/2025 08:19</t>
+          <t>11/08/2025 05:31</t>
         </is>
       </c>
       <c r="C9" s="15">
-        <f>hyperlink("notas fiscal/20250623_082034.jpg", "20250623_082034.jpg")</f>
+        <f>hyperlink("notas fiscal/20250811_211802.jpg", "20250811_211802.jpg")</f>
         <v/>
       </c>
       <c r="D9" s="16" t="n">
-        <v>10.99</v>
+        <v>37.9</v>
       </c>
     </row>
     <row r="10" ht="17.35" customFormat="1" customHeight="1" s="6">
       <c r="A10" s="14" t="inlineStr">
         <is>
-          <t>comercial iguatemi ltda- me</t>
+          <t>restaurante moinho ltda</t>
         </is>
       </c>
       <c r="B10" s="14" t="inlineStr">
         <is>
-          <t>23/06/2025 10:04</t>
+          <t>11/08/2025 12:51</t>
         </is>
       </c>
       <c r="C10" s="15">
-        <f>hyperlink("notas fiscal/20250623_100731.jpg", "20250623_100731.jpg")</f>
+        <f>hyperlink("notas fiscal/20250811_211646.jpg", "20250811_211646.jpg")</f>
         <v/>
       </c>
       <c r="D10" s="16" t="n">
-        <v>16</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" ht="17.35" customFormat="1" customHeight="1" s="6">
-      <c r="A11" s="14" t="inlineStr">
-        <is>
-          <t>panificadora amigos ltda</t>
-        </is>
-      </c>
-      <c r="B11" s="14" t="inlineStr">
-        <is>
-          <t>24/06/2025 07:36</t>
-        </is>
-      </c>
-      <c r="C11" s="15">
-        <f>hyperlink("notas fiscal/20250624_073800_1yl5PSC.jpg", "20250624_073800_1yl5PSC.jpg")</f>
+      <c r="A11" s="17" t="inlineStr">
+        <is>
+          <t>TOTAL</t>
+        </is>
+      </c>
+      <c r="B11" s="18" t="n"/>
+      <c r="C11" s="18" t="n"/>
+      <c r="D11" s="14">
+        <f>sum(D9:D10)</f>
         <v/>
       </c>
-      <c r="D11" s="16" t="n">
-        <v>14.5</v>
-      </c>
     </row>
     <row r="12" ht="17.35" customFormat="1" customHeight="1" s="6">
-      <c r="A12" s="14" t="inlineStr">
-        <is>
-          <t>bar e restaurante dona nilza</t>
-        </is>
-      </c>
-      <c r="B12" s="14" t="inlineStr">
-        <is>
-          <t>24/06/2025 12:22</t>
-        </is>
-      </c>
-      <c r="C12" s="15">
-        <f>hyperlink("notas fiscal/20250628_090221.jpg", "20250628_090221.jpg")</f>
-        <v/>
-      </c>
-      <c r="D12" s="16" t="n">
-        <v>27.5</v>
-      </c>
+      <c r="A12" s="19" t="n"/>
+      <c r="B12" s="19" t="n"/>
+      <c r="C12" s="19" t="n"/>
+      <c r="D12" s="19" t="n"/>
     </row>
     <row r="13" ht="17.35" customFormat="1" customHeight="1" s="6">
-      <c r="A13" s="14" t="inlineStr">
-        <is>
-          <t>dma distribuidora s/a</t>
-        </is>
-      </c>
-      <c r="B13" s="14" t="inlineStr">
-        <is>
-          <t>24/06/2025 17:46</t>
-        </is>
-      </c>
-      <c r="C13" s="15">
-        <f>hyperlink("notas fiscal/20250624_184701.jpg", "20250624_184701.jpg")</f>
-        <v/>
-      </c>
-      <c r="D13" s="16" t="n">
-        <v>29.78</v>
-      </c>
+      <c r="A13" s="17" t="inlineStr">
+        <is>
+          <t>Descricão Do Adiantamento</t>
+        </is>
+      </c>
+      <c r="B13" s="18" t="n"/>
+      <c r="C13" s="18" t="n"/>
+      <c r="D13" s="18" t="n"/>
     </row>
     <row r="14" ht="17.35" customFormat="1" customHeight="1" s="6">
-      <c r="A14" s="14" t="inlineStr">
-        <is>
-          <t>bar e restaurante dona nilza</t>
-        </is>
-      </c>
-      <c r="B14" s="14" t="inlineStr">
-        <is>
-          <t>25/06/2025 12:51</t>
-        </is>
-      </c>
-      <c r="C14" s="15">
-        <f>hyperlink("notas fiscal/20250625_125327.jpg", "20250625_125327.jpg")</f>
-        <v/>
-      </c>
-      <c r="D14" s="16" t="n">
-        <v>32.49</v>
+      <c r="A14" s="17" t="inlineStr">
+        <is>
+          <t>Descrição</t>
+        </is>
+      </c>
+      <c r="B14" s="17" t="inlineStr">
+        <is>
+          <t>Data</t>
+        </is>
+      </c>
+      <c r="C14" s="17" t="inlineStr">
+        <is>
+          <t>Comprovante</t>
+        </is>
+      </c>
+      <c r="D14" s="17" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
       </c>
     </row>
     <row r="15" ht="17.35" customFormat="1" customHeight="1" s="6">
       <c r="A15" s="14" t="inlineStr">
         <is>
-          <t>bar e restaurante dona nilza</t>
+          <t>transferênciarecebida</t>
         </is>
       </c>
       <c r="B15" s="14" t="inlineStr">
         <is>
-          <t>26/06/2025 12:16</t>
+          <t>08/08/2025 10:49</t>
         </is>
       </c>
       <c r="C15" s="15">
-        <f>hyperlink("notas fiscal/20250626_121759.jpg", "20250626_121759.jpg")</f>
+        <f>hyperlink("notas fiscal/15692.jpg", "15692.jpg")</f>
         <v/>
       </c>
       <c r="D15" s="16" t="n">
-        <v>30.51</v>
+        <v>500</v>
       </c>
     </row>
     <row r="16" ht="17.35" customFormat="1" customHeight="1" s="6">
-      <c r="A16" s="14" t="inlineStr">
-        <is>
-          <t>lanchonete sabor e saúde</t>
-        </is>
-      </c>
-      <c r="B16" s="14" t="inlineStr">
-        <is>
-          <t>26/06/2025 18:00</t>
-        </is>
-      </c>
-      <c r="C16" s="15">
-        <f>hyperlink("notas fiscal/20250626_211609_pT9iyyC.jpg", "20250626_211609_pT9iyyC.jpg")</f>
+      <c r="A16" s="19" t="n"/>
+      <c r="B16" s="19" t="n"/>
+      <c r="C16" s="19" t="n"/>
+      <c r="D16" s="19" t="n"/>
+    </row>
+    <row r="17" ht="17.35" customFormat="1" customHeight="1" s="6">
+      <c r="A17" s="17" t="inlineStr">
+        <is>
+          <t>Receber</t>
+        </is>
+      </c>
+      <c r="B17" s="18" t="n"/>
+      <c r="C17" s="17" t="inlineStr">
+        <is>
+          <t>Devolver</t>
+        </is>
+      </c>
+      <c r="D17" s="18" t="n"/>
+    </row>
+    <row r="18" ht="17.35" customFormat="1" customHeight="1" s="6">
+      <c r="A18" s="16">
+        <f>if(sum(D15:D15) - D11 &lt;0, D11 - sum(D15:D15), 0)</f>
         <v/>
       </c>
-      <c r="D16" s="16" t="n">
-        <v>6.5</v>
-      </c>
-    </row>
-    <row r="17" ht="17.35" customFormat="1" customHeight="1" s="6">
-      <c r="A17" s="14" t="inlineStr">
-        <is>
-          <t>bar e restaurante dona nilza</t>
-        </is>
-      </c>
-      <c r="B17" s="14" t="inlineStr">
-        <is>
-          <t>27/06/2025 12:14</t>
-        </is>
-      </c>
-      <c r="C17" s="15">
-        <f>hyperlink("notas fiscal/20250628_085259.jpg", "20250628_085259.jpg")</f>
+      <c r="B18" s="18" t="n"/>
+      <c r="C18" s="16">
+        <f>if(sum(D15:D15) - D11&lt;0, 0, sum(D15:D15) -  D11)</f>
         <v/>
       </c>
-      <c r="D17" s="16" t="n">
-        <v>32.49</v>
-      </c>
-    </row>
-    <row r="18" ht="17.35" customFormat="1" customHeight="1" s="6">
-      <c r="A18" s="14" t="inlineStr">
-        <is>
-          <t>mercado bh, mercado epa,  ifood</t>
-        </is>
-      </c>
-      <c r="B18" s="14" t="inlineStr">
-        <is>
-          <t>27/06/2025 20:14</t>
-        </is>
-      </c>
-      <c r="C18" s="15">
-        <f>hyperlink("notas fiscal/IMG-20250628-WA0004.jpg", "IMG-20250628-WA0004.jpg")</f>
-        <v/>
-      </c>
-      <c r="D18" s="16" t="n">
-        <v>268.89</v>
-      </c>
+      <c r="D18" s="18" t="n"/>
     </row>
     <row r="19" ht="17.35" customFormat="1" customHeight="1" s="6">
-      <c r="A19" s="14" t="inlineStr">
-        <is>
-          <t>jaqueline oliveira de melo</t>
-        </is>
-      </c>
-      <c r="B19" s="14" t="inlineStr">
-        <is>
-          <t>28/06/2025 12:26</t>
-        </is>
-      </c>
-      <c r="C19" s="15">
-        <f>hyperlink("notas fiscal/20250623_122829.jpg", "20250623_122829.jpg")</f>
-        <v/>
-      </c>
-      <c r="D19" s="16" t="n">
-        <v>21.22</v>
-      </c>
+      <c r="A19" s="19" t="n"/>
+      <c r="B19" s="19" t="n"/>
+      <c r="C19" s="19" t="n"/>
+      <c r="D19" s="19" t="n"/>
     </row>
     <row r="20" ht="17.35" customFormat="1" customHeight="1" s="6">
-      <c r="A20" s="14" t="inlineStr">
-        <is>
-          <t>mercado bh</t>
-        </is>
-      </c>
-      <c r="B20" s="14" t="inlineStr">
-        <is>
-          <t>28/06/2025 15:16</t>
-        </is>
-      </c>
-      <c r="C20" s="15">
-        <f>hyperlink("notas fiscal/IMG-20250628-WA0005.jpg", "IMG-20250628-WA0005.jpg")</f>
-        <v/>
-      </c>
-      <c r="D20" s="16" t="n">
-        <v>51.54</v>
+      <c r="A20" s="19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Apucarana, 11 de agosto de 2025 </t>
+        </is>
       </c>
     </row>
     <row r="21" ht="17.35" customFormat="1" customHeight="1" s="6">
-      <c r="A21" s="14" t="inlineStr">
-        <is>
-          <t>jantar</t>
-        </is>
-      </c>
-      <c r="B21" s="14" t="inlineStr">
-        <is>
-          <t>28/06/2025 21:17</t>
-        </is>
-      </c>
-      <c r="C21" s="15">
-        <f>hyperlink("notas fiscal/IMG-20250628-WA0010_gO3PprR.jpg", "IMG-20250628-WA0010_gO3PprR.jpg")</f>
-        <v/>
-      </c>
-      <c r="D21" s="16" t="n">
-        <v>71.13</v>
-      </c>
+      <c r="A21" s="19" t="n"/>
+      <c r="B21" s="19" t="n"/>
+      <c r="C21" s="19" t="n"/>
+      <c r="D21" s="19" t="n"/>
     </row>
     <row r="22" ht="17.35" customHeight="1" s="8">
-      <c r="A22" s="14" t="inlineStr">
-        <is>
-          <t>bar e restaurante dona nilza</t>
-        </is>
-      </c>
-      <c r="B22" s="14" t="inlineStr">
-        <is>
-          <t>30/06/2025 12:34</t>
-        </is>
-      </c>
-      <c r="C22" s="15">
-        <f>hyperlink("notas fiscal/20250630_123543.jpg", "20250630_123543.jpg")</f>
-        <v/>
-      </c>
-      <c r="D22" s="16" t="n">
-        <v>31</v>
+      <c r="A22" s="19" t="inlineStr">
+        <is>
+          <t>__________________________________</t>
+        </is>
+      </c>
+      <c r="C22" s="19" t="inlineStr">
+        <is>
+          <t>__________________________________</t>
+        </is>
       </c>
     </row>
     <row r="23" ht="17.35" customHeight="1" s="8">
-      <c r="A23" s="14" t="inlineStr">
-        <is>
-          <t>jantar</t>
-        </is>
-      </c>
-      <c r="B23" s="14" t="inlineStr">
-        <is>
-          <t>30/06/2025 20:06</t>
-        </is>
-      </c>
-      <c r="C23" s="15">
-        <f>hyperlink("notas fiscal/IMG-20250701-WA0017.jpg", "IMG-20250701-WA0017.jpg")</f>
-        <v/>
-      </c>
-      <c r="D23" s="16" t="n">
-        <v>31.65</v>
-      </c>
+      <c r="A23" s="19" t="n"/>
+      <c r="C23" s="19" t="n"/>
     </row>
     <row r="24" ht="17.35" customHeight="1" s="8">
-      <c r="A24" s="14" t="inlineStr">
-        <is>
-          <t>bar e restaurante dona nilza</t>
-        </is>
-      </c>
-      <c r="B24" s="14" t="inlineStr">
-        <is>
-          <t>01/07/2025 12:37</t>
-        </is>
-      </c>
-      <c r="C24" s="15">
-        <f>hyperlink("notas fiscal/20250702_232526.jpg", "20250702_232526.jpg")</f>
-        <v/>
-      </c>
-      <c r="D24" s="16" t="n">
-        <v>25.02</v>
-      </c>
+      <c r="A24" s="19" t="n"/>
+      <c r="B24" s="19" t="n"/>
+      <c r="C24" s="19" t="n"/>
+      <c r="D24" s="19" t="n"/>
     </row>
     <row r="25" ht="17.35" customHeight="1" s="8">
-      <c r="A25" s="14" t="inlineStr">
-        <is>
-          <t>churrascaria boi na brasa</t>
-        </is>
-      </c>
-      <c r="B25" s="14" t="inlineStr">
-        <is>
-          <t>02/07/2025 06:44</t>
-        </is>
-      </c>
-      <c r="C25" s="15">
-        <f>hyperlink("notas fiscal/20250702_230555.jpg", "20250702_230555.jpg")</f>
-        <v/>
-      </c>
-      <c r="D25" s="16" t="n">
-        <v>15</v>
-      </c>
+      <c r="A25" s="19" t="n"/>
+      <c r="B25" s="19" t="n"/>
+      <c r="C25" s="19" t="n"/>
+      <c r="D25" s="19" t="n"/>
     </row>
     <row r="26" ht="17.35" customHeight="1" s="8">
-      <c r="A26" s="14" t="inlineStr">
-        <is>
-          <t>doces queijos iguatemy</t>
-        </is>
-      </c>
-      <c r="B26" s="14" t="inlineStr">
-        <is>
-          <t>02/07/2025 07:19</t>
-        </is>
-      </c>
-      <c r="C26" s="15">
-        <f>hyperlink("notas fiscal/20250702_230408.jpg", "20250702_230408.jpg")</f>
-        <v/>
-      </c>
-      <c r="D26" s="16" t="n">
-        <v>73.04000000000001</v>
-      </c>
+      <c r="A26" s="19" t="n"/>
+      <c r="B26" s="19" t="n"/>
+      <c r="C26" s="19" t="n"/>
+      <c r="D26" s="19" t="n"/>
     </row>
     <row r="27" ht="17.35" customHeight="1" s="8">
-      <c r="A27" s="14" t="inlineStr">
-        <is>
-          <t>restaurante cazulao</t>
-        </is>
-      </c>
-      <c r="B27" s="14" t="inlineStr">
-        <is>
-          <t>02/07/2025 10:48</t>
-        </is>
-      </c>
-      <c r="C27" s="15">
-        <f>hyperlink("notas fiscal/20250702_225912_ASJ9Sfd.jpg", "20250702_225912_ASJ9Sfd.jpg")</f>
-        <v/>
-      </c>
-      <c r="D27" s="16" t="n">
-        <v>18</v>
-      </c>
+      <c r="A27" s="19" t="n"/>
+      <c r="B27" s="19" t="n"/>
+      <c r="C27" s="19" t="n"/>
+      <c r="D27" s="19" t="n"/>
     </row>
     <row r="28" ht="17.35" customHeight="1" s="8">
-      <c r="A28" s="14" t="inlineStr">
-        <is>
-          <t>churrascaria tucuman ltda</t>
-        </is>
-      </c>
-      <c r="B28" s="14" t="inlineStr">
-        <is>
-          <t>02/07/2025 13:52</t>
-        </is>
-      </c>
-      <c r="C28" s="15">
-        <f>hyperlink("notas fiscal/20250702_225517.jpg", "20250702_225517.jpg")</f>
-        <v/>
-      </c>
-      <c r="D28" s="16" t="n">
-        <v>23.9</v>
-      </c>
+      <c r="A28" s="19" t="n"/>
+      <c r="B28" s="19" t="n"/>
+      <c r="C28" s="19" t="n"/>
+      <c r="D28" s="19" t="n"/>
     </row>
     <row r="29" ht="17.35" customHeight="1" s="8">
-      <c r="A29" s="17" t="inlineStr">
-        <is>
-          <t>TOTAL</t>
-        </is>
-      </c>
-      <c r="B29" s="18" t="n"/>
-      <c r="C29" s="18" t="n"/>
-      <c r="D29" s="14">
-        <f>sum(D9:D28)</f>
-        <v/>
-      </c>
+      <c r="A29" s="19" t="n"/>
+      <c r="B29" s="19" t="n"/>
+      <c r="C29" s="19" t="n"/>
+      <c r="D29" s="19" t="n"/>
     </row>
     <row r="30" ht="17.35" customHeight="1" s="8">
       <c r="A30" s="19" t="n"/>
@@ -904,74 +721,28 @@
       <c r="D30" s="19" t="n"/>
     </row>
     <row r="31" ht="17.35" customHeight="1" s="8">
-      <c r="A31" s="17" t="inlineStr">
-        <is>
-          <t>Descricão Do Adiantamento</t>
-        </is>
-      </c>
-      <c r="B31" s="18" t="n"/>
-      <c r="C31" s="18" t="n"/>
-      <c r="D31" s="18" t="n"/>
+      <c r="A31" s="19" t="n"/>
+      <c r="B31" s="19" t="n"/>
+      <c r="C31" s="19" t="n"/>
+      <c r="D31" s="19" t="n"/>
     </row>
     <row r="32" ht="17.35" customHeight="1" s="8">
-      <c r="A32" s="17" t="inlineStr">
-        <is>
-          <t>Descrição</t>
-        </is>
-      </c>
-      <c r="B32" s="17" t="inlineStr">
-        <is>
-          <t>Data</t>
-        </is>
-      </c>
-      <c r="C32" s="17" t="inlineStr">
-        <is>
-          <t>Comprovante</t>
-        </is>
-      </c>
-      <c r="D32" s="17" t="inlineStr">
-        <is>
-          <t>Value</t>
-        </is>
-      </c>
+      <c r="A32" s="19" t="n"/>
+      <c r="B32" s="19" t="n"/>
+      <c r="C32" s="19" t="n"/>
+      <c r="D32" s="19" t="n"/>
     </row>
     <row r="33" ht="17.35" customHeight="1" s="8">
-      <c r="A33" s="14" t="inlineStr">
-        <is>
-          <t>transferencia recebida</t>
-        </is>
-      </c>
-      <c r="B33" s="14" t="inlineStr">
-        <is>
-          <t>20/06/2025 08:49</t>
-        </is>
-      </c>
-      <c r="C33" s="15">
-        <f>hyperlink("notas fiscal/IMG-20250629-WA0010_ux4VgRy.jpg", "IMG-20250629-WA0010_ux4VgRy.jpg")</f>
-        <v/>
-      </c>
-      <c r="D33" s="16" t="n">
-        <v>800</v>
-      </c>
+      <c r="A33" s="19" t="n"/>
+      <c r="B33" s="19" t="n"/>
+      <c r="C33" s="19" t="n"/>
+      <c r="D33" s="19" t="n"/>
     </row>
     <row r="34" ht="17.35" customHeight="1" s="8">
-      <c r="A34" s="14" t="inlineStr">
-        <is>
-          <t>transferencia recebida</t>
-        </is>
-      </c>
-      <c r="B34" s="14" t="inlineStr">
-        <is>
-          <t>30/06/2025 11:05</t>
-        </is>
-      </c>
-      <c r="C34" s="15">
-        <f>hyperlink("notas fiscal/IMG-20250701-WA0016_eCzmQzQ.jpg", "IMG-20250701-WA0016_eCzmQzQ.jpg")</f>
-        <v/>
-      </c>
-      <c r="D34" s="16" t="n">
-        <v>700</v>
-      </c>
+      <c r="A34" s="19" t="n"/>
+      <c r="B34" s="19" t="n"/>
+      <c r="C34" s="19" t="n"/>
+      <c r="D34" s="19" t="n"/>
     </row>
     <row r="35" ht="17.35" customHeight="1" s="8">
       <c r="A35" s="19" t="n"/>
@@ -980,71 +751,31 @@
       <c r="D35" s="19" t="n"/>
     </row>
     <row r="36" ht="17.35" customHeight="1" s="8">
-      <c r="A36" s="17" t="inlineStr">
-        <is>
-          <t>Receber</t>
-        </is>
-      </c>
-      <c r="B36" s="18" t="n"/>
-      <c r="C36" s="17" t="inlineStr">
-        <is>
-          <t>Devolver</t>
-        </is>
-      </c>
-      <c r="D36" s="18" t="n"/>
-    </row>
-    <row r="37">
-      <c r="A37" s="20">
-        <f>if(sum(D33:D34) - D29 &lt;0, D29 - sum(D33:D34), 0)</f>
-        <v/>
-      </c>
-      <c r="B37" s="18" t="n"/>
-      <c r="C37" s="20">
-        <f>if(sum(D33:D34) - D29&lt;0, 0, sum(D33:D34) -  D29)</f>
-        <v/>
-      </c>
-      <c r="D37" s="18" t="n"/>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Apucarana, 03 de julho de 2025 </t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>__________________________________</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>__________________________________</t>
-        </is>
-      </c>
-    </row>
-    <row r="42"/>
+      <c r="A36" s="19" t="n"/>
+      <c r="B36" s="19" t="n"/>
+      <c r="C36" s="19" t="n"/>
+      <c r="D36" s="19" t="n"/>
+    </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A31:D31"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="A39:D39"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="A18:B18"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="B4:D4"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="C36:D36"/>
     <mergeCell ref="A7:D7"/>
-    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="C18:D18"/>
     <mergeCell ref="C3:D3"/>
   </mergeCells>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>

</xml_diff>